<commit_message>
Add files to begin separating data collection and plotting
</commit_message>
<xml_diff>
--- a/data/GolfData.xlsx
+++ b/data/GolfData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\Golf\GolfStats\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Apps\GolfStats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D3BAF0-19E6-4E31-A302-077939333E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B07D92-964B-49FE-AD84-EB3E5EE06161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C4BA5778-8140-4272-B97C-07E35F2520D6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4BA5778-8140-4272-B97C-07E35F2520D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Score Cards" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -1134,8 +1134,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}" name="Table1" displayName="Table1" ref="A1:W3" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69">
-  <autoFilter ref="A1:W3" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}" name="Table1" displayName="Table1" ref="A1:W4" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69">
+  <autoFilter ref="A1:W4" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{6036417A-52C2-4AF8-9A0D-25AEE607F48A}" name="Course" dataDxfId="68"/>
     <tableColumn id="2" xr3:uid="{AE08F17B-78CF-43B6-86B1-7635DA793064}" name="Date" dataDxfId="67"/>
@@ -1518,23 +1518,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838B056B-02E7-4106-A28B-369A087ADF9A}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="1" customWidth="1"/>
-    <col min="3" max="21" width="8.88671875" style="1"/>
-    <col min="22" max="22" width="11.88671875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="12.33203125" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
+    <col min="3" max="21" width="8.85546875" style="1"/>
+    <col min="22" max="22" width="11.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1745,6 +1745,77 @@
       </c>
       <c r="W3" s="1">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45633</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>6</v>
+      </c>
+      <c r="L4" s="1">
+        <v>5</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1">
+        <v>6</v>
+      </c>
+      <c r="O4" s="1">
+        <v>4</v>
+      </c>
+      <c r="P4" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>3</v>
+      </c>
+      <c r="R4" s="1">
+        <v>6</v>
+      </c>
+      <c r="S4" s="1">
+        <v>4</v>
+      </c>
+      <c r="T4" s="1">
+        <v>6</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
+        <v>34</v>
+      </c>
+      <c r="W4" s="1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1760,15 +1831,15 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:S2"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1827,7 +1898,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1902,12 +1973,12 @@
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1966,7 +2037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Add scores from 28 DEC 2024
</commit_message>
<xml_diff>
--- a/data/GolfData.xlsx
+++ b/data/GolfData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Apps\GolfStats\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Apps\GolfStats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B07D92-964B-49FE-AD84-EB3E5EE06161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D177E00F-B9BB-4059-A6FD-F22A3E587D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4BA5778-8140-4272-B97C-07E35F2520D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C4BA5778-8140-4272-B97C-07E35F2520D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Score Cards" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -1134,8 +1134,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}" name="Table1" displayName="Table1" ref="A1:W4" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69">
-  <autoFilter ref="A1:W4" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}" name="Table1" displayName="Table1" ref="A1:W5" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69">
+  <autoFilter ref="A1:W5" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{6036417A-52C2-4AF8-9A0D-25AEE607F48A}" name="Course" dataDxfId="68"/>
     <tableColumn id="2" xr3:uid="{AE08F17B-78CF-43B6-86B1-7635DA793064}" name="Date" dataDxfId="67"/>
@@ -1518,23 +1518,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838B056B-02E7-4106-A28B-369A087ADF9A}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
-    <col min="3" max="21" width="8.85546875" style="1"/>
-    <col min="22" max="22" width="11.85546875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="12.28515625" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="1" customWidth="1"/>
+    <col min="3" max="21" width="8.88671875" style="1"/>
+    <col min="22" max="22" width="11.88671875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1816,6 +1816,77 @@
       </c>
       <c r="W4" s="1">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45654</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1">
+        <v>6</v>
+      </c>
+      <c r="J5" s="1">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>3</v>
+      </c>
+      <c r="M5" s="1">
+        <v>4</v>
+      </c>
+      <c r="N5" s="1">
+        <v>5</v>
+      </c>
+      <c r="O5" s="1">
+        <v>4</v>
+      </c>
+      <c r="P5" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>6</v>
+      </c>
+      <c r="R5" s="1">
+        <v>6</v>
+      </c>
+      <c r="S5" s="1">
+        <v>4</v>
+      </c>
+      <c r="T5" s="1">
+        <v>4</v>
+      </c>
+      <c r="U5" s="1">
+        <v>4</v>
+      </c>
+      <c r="V5" s="1">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1834,12 +1905,12 @@
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1898,7 +1969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1973,12 +2044,12 @@
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2037,7 +2108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Update app to have first golf graph
</commit_message>
<xml_diff>
--- a/data/GolfData.xlsx
+++ b/data/GolfData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Apps\GolfStats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D177E00F-B9BB-4059-A6FD-F22A3E587D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AB3C8E-6180-4326-AC1E-BDCE8D4F3783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C4BA5778-8140-4272-B97C-07E35F2520D6}"/>
   </bookViews>

</xml_diff>

<commit_message>
Update data for 28 June 2025
</commit_message>
<xml_diff>
--- a/data/GolfData.xlsx
+++ b/data/GolfData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Apps\GolfStats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F883109-DC7D-4870-99FA-807B27A309BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EF2778-B3BE-4B96-B8C3-0BE6D901FE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C4BA5778-8140-4272-B97C-07E35F2520D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -1178,8 +1178,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}" name="Table1" displayName="Table1" ref="A1:W11" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71">
-  <autoFilter ref="A1:W11" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}" name="Table1" displayName="Table1" ref="A1:W12" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71">
+  <autoFilter ref="A1:W12" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{6036417A-52C2-4AF8-9A0D-25AEE607F48A}" name="Course" dataDxfId="70"/>
     <tableColumn id="2" xr3:uid="{AE08F17B-78CF-43B6-86B1-7635DA793064}" name="Date" dataDxfId="69"/>
@@ -1564,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838B056B-02E7-4106-A28B-369A087ADF9A}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2359,6 +2359,77 @@
       </c>
       <c r="W11" s="1">
         <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45836</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1">
+        <v>4</v>
+      </c>
+      <c r="I12" s="1">
+        <v>6</v>
+      </c>
+      <c r="J12" s="1">
+        <v>4</v>
+      </c>
+      <c r="K12" s="1">
+        <v>4</v>
+      </c>
+      <c r="L12" s="1">
+        <v>5</v>
+      </c>
+      <c r="M12" s="1">
+        <v>4</v>
+      </c>
+      <c r="N12" s="1">
+        <v>8</v>
+      </c>
+      <c r="O12" s="1">
+        <v>7</v>
+      </c>
+      <c r="P12" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>5</v>
+      </c>
+      <c r="R12" s="1">
+        <v>5</v>
+      </c>
+      <c r="S12" s="1">
+        <v>4</v>
+      </c>
+      <c r="T12" s="1">
+        <v>4</v>
+      </c>
+      <c r="U12" s="1">
+        <v>3</v>
+      </c>
+      <c r="V12" s="1">
+        <v>42</v>
+      </c>
+      <c r="W12" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V1.5.3 - add new numeric metrics.
</commit_message>
<xml_diff>
--- a/data/GolfData.xlsx
+++ b/data/GolfData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Apps\GolfStats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76ED35FD-D1F0-4D3B-8CA6-74A3070D367B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C87DCD9-D48F-4253-B1B7-F48F002BA118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C4BA5778-8140-4272-B97C-07E35F2520D6}"/>
+    <workbookView xWindow="1170" yWindow="2610" windowWidth="20355" windowHeight="12285" xr2:uid="{C4BA5778-8140-4272-B97C-07E35F2520D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Score Cards" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Honey Bee</t>
+  </si>
+  <si>
+    <t>Cypress Point</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -224,6 +227,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,8 +1187,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}" name="Table1" displayName="Table1" ref="A1:W15" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71">
-  <autoFilter ref="A1:W15" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}" name="Table1" displayName="Table1" ref="A1:W16" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71">
+  <autoFilter ref="A1:W16" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{6036417A-52C2-4AF8-9A0D-25AEE607F48A}" name="Course" dataDxfId="70"/>
     <tableColumn id="2" xr3:uid="{AE08F17B-78CF-43B6-86B1-7635DA793064}" name="Date" dataDxfId="69"/>
@@ -1241,8 +1247,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E23CC1EA-99BC-4242-AF8E-4EFD850D2CFF}" name="Table24" displayName="Table24" ref="A1:U3" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21">
-  <autoFilter ref="A1:U3" xr:uid="{E23CC1EA-99BC-4242-AF8E-4EFD850D2CFF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E23CC1EA-99BC-4242-AF8E-4EFD850D2CFF}" name="Table24" displayName="Table24" ref="A1:U4" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21">
+  <autoFilter ref="A1:U4" xr:uid="{E23CC1EA-99BC-4242-AF8E-4EFD850D2CFF}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{CFEBEA66-C11E-40EA-9B1C-519F8D6D5A4D}" name="Course" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{E3A55B99-6240-4A04-9BEC-04FB4FD27D1A}" name="1" dataDxfId="19"/>
@@ -1567,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838B056B-02E7-4106-A28B-369A087ADF9A}">
-  <dimension ref="A1:W15"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2646,6 +2652,77 @@
       </c>
       <c r="W15" s="1">
         <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2">
+        <v>45899</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>7</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1">
+        <v>6</v>
+      </c>
+      <c r="I16" s="1">
+        <v>5</v>
+      </c>
+      <c r="J16" s="1">
+        <v>6</v>
+      </c>
+      <c r="K16" s="1">
+        <v>4</v>
+      </c>
+      <c r="L16" s="1">
+        <v>5</v>
+      </c>
+      <c r="M16" s="1">
+        <v>3</v>
+      </c>
+      <c r="N16" s="1">
+        <v>4</v>
+      </c>
+      <c r="O16" s="1">
+        <v>5</v>
+      </c>
+      <c r="P16" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>4</v>
+      </c>
+      <c r="R16" s="1">
+        <v>4</v>
+      </c>
+      <c r="S16" s="1">
+        <v>5</v>
+      </c>
+      <c r="T16" s="1">
+        <v>6</v>
+      </c>
+      <c r="U16" s="1">
+        <v>5</v>
+      </c>
+      <c r="V16" s="1">
+        <v>37</v>
+      </c>
+      <c r="W16" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2856,10 +2933,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534A788D-C5D7-487E-983A-A68219D7D8C3}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3062,6 +3139,71 @@
         <v>121</v>
       </c>
     </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="7">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>5</v>
+      </c>
+      <c r="F4" s="7">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7">
+        <v>4</v>
+      </c>
+      <c r="H4" s="7">
+        <v>4</v>
+      </c>
+      <c r="I4" s="7">
+        <v>5</v>
+      </c>
+      <c r="J4" s="7">
+        <v>3</v>
+      </c>
+      <c r="K4" s="7">
+        <v>4</v>
+      </c>
+      <c r="L4" s="7">
+        <v>3</v>
+      </c>
+      <c r="M4" s="7">
+        <v>4</v>
+      </c>
+      <c r="N4" s="7">
+        <v>4</v>
+      </c>
+      <c r="O4" s="7">
+        <v>5</v>
+      </c>
+      <c r="P4" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>4</v>
+      </c>
+      <c r="R4" s="7">
+        <v>3</v>
+      </c>
+      <c r="S4" s="7">
+        <v>5</v>
+      </c>
+      <c r="T4" s="7">
+        <v>69</v>
+      </c>
+      <c r="U4" s="7">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Oct 04 2025 score update & clean
</commit_message>
<xml_diff>
--- a/data/GolfData.xlsx
+++ b/data/GolfData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Apps\GolfStats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C87DCD9-D48F-4253-B1B7-F48F002BA118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F4F171-DFBE-4357-BEF0-0DA31174CAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="2610" windowWidth="20355" windowHeight="12285" xr2:uid="{C4BA5778-8140-4272-B97C-07E35F2520D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C4BA5778-8140-4272-B97C-07E35F2520D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Score Cards" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -207,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,9 +227,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1187,8 +1184,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}" name="Table1" displayName="Table1" ref="A1:W16" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71">
-  <autoFilter ref="A1:W16" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}" name="Table1" displayName="Table1" ref="A1:W17" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71">
+  <autoFilter ref="A1:W17" xr:uid="{67CDCE95-7C63-4EE1-A07D-718040E657E9}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{6036417A-52C2-4AF8-9A0D-25AEE607F48A}" name="Course" dataDxfId="70"/>
     <tableColumn id="2" xr3:uid="{AE08F17B-78CF-43B6-86B1-7635DA793064}" name="Date" dataDxfId="69"/>
@@ -1573,10 +1570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838B056B-02E7-4106-A28B-369A087ADF9A}">
-  <dimension ref="A1:W16"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2723,6 +2720,77 @@
       </c>
       <c r="W16" s="1">
         <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45934</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6</v>
+      </c>
+      <c r="G17" s="1">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1">
+        <v>7</v>
+      </c>
+      <c r="J17" s="1">
+        <v>5</v>
+      </c>
+      <c r="K17" s="1">
+        <v>4</v>
+      </c>
+      <c r="L17" s="1">
+        <v>4</v>
+      </c>
+      <c r="M17" s="1">
+        <v>7</v>
+      </c>
+      <c r="N17" s="1">
+        <v>4</v>
+      </c>
+      <c r="O17" s="1">
+        <v>3</v>
+      </c>
+      <c r="P17" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>4</v>
+      </c>
+      <c r="R17" s="1">
+        <v>5</v>
+      </c>
+      <c r="S17" s="1">
+        <v>3</v>
+      </c>
+      <c r="T17" s="1">
+        <v>3</v>
+      </c>
+      <c r="U17" s="1">
+        <v>3</v>
+      </c>
+      <c r="V17" s="1">
+        <v>31</v>
+      </c>
+      <c r="W17" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3143,64 +3211,64 @@
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="7">
-        <v>4</v>
-      </c>
-      <c r="C4" s="7">
-        <v>5</v>
-      </c>
-      <c r="D4" s="7">
-        <v>3</v>
-      </c>
-      <c r="E4" s="7">
-        <v>5</v>
-      </c>
-      <c r="F4" s="7">
-        <v>3</v>
-      </c>
-      <c r="G4" s="7">
-        <v>4</v>
-      </c>
-      <c r="H4" s="7">
-        <v>4</v>
-      </c>
-      <c r="I4" s="7">
-        <v>5</v>
-      </c>
-      <c r="J4" s="7">
-        <v>3</v>
-      </c>
-      <c r="K4" s="7">
-        <v>4</v>
-      </c>
-      <c r="L4" s="7">
-        <v>3</v>
-      </c>
-      <c r="M4" s="7">
-        <v>4</v>
-      </c>
-      <c r="N4" s="7">
-        <v>4</v>
-      </c>
-      <c r="O4" s="7">
-        <v>5</v>
-      </c>
-      <c r="P4" s="7">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>4</v>
-      </c>
-      <c r="R4" s="7">
-        <v>3</v>
-      </c>
-      <c r="S4" s="7">
-        <v>5</v>
-      </c>
-      <c r="T4" s="7">
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1">
+        <v>5</v>
+      </c>
+      <c r="J4" s="1">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1">
+        <v>4</v>
+      </c>
+      <c r="N4" s="1">
+        <v>4</v>
+      </c>
+      <c r="O4" s="1">
+        <v>5</v>
+      </c>
+      <c r="P4" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>4</v>
+      </c>
+      <c r="R4" s="1">
+        <v>3</v>
+      </c>
+      <c r="S4" s="1">
+        <v>5</v>
+      </c>
+      <c r="T4" s="1">
         <v>69</v>
       </c>
-      <c r="U4" s="7">
+      <c r="U4" s="1">
         <v>118</v>
       </c>
     </row>

</xml_diff>